<commit_message>
i add reset printer part fun
</commit_message>
<xml_diff>
--- a/printer.xlsx
+++ b/printer.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -898,6 +898,105 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>d184b53b-4e1c-4a33-99bf-f1ae7a652587</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Duable Face</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>100</v>
+      </c>
+      <c r="E17" t="n">
+        <v>15</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>21:16:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>53ad640e-13ca-4935-b419-d47ed9b1373e</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Duable Face</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" t="n">
+        <v>15</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>21:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>496ebab3-efbf-4798-b5d3-03cf252cb766</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Duable Face</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E19" t="n">
+        <v>15</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>21:31:33</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix issues in the savePrinterData function
</commit_message>
<xml_diff>
--- a/printer.xlsx
+++ b/printer.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,6 +491,237 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>46cea3b9-bf3a-400c-a9ca-f07bc02c51f0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Waste</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>17:23:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>c0d653bf-2f1a-4cfa-988f-9ee6b267ef45</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Waste</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>17:45:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>229acf0c-779f-434d-a864-34fde3ed54e9</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>17:45:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>0535ef63-cd48-482b-806e-b8e7360c32ac</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>17:51:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1899b5d8-72a6-4f60-91fc-a9c68866dd90</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>17:52:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>006ffc8f-2e6b-4a91-b27d-4b7a650f632d</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1234</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>17:54:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>3d7a2e09-c12c-49df-86b9-f90c2a8fd76f</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ram</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10101</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>17:56:11</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
i add delet functionality in the printer section
</commit_message>
<xml_diff>
--- a/printer.xlsx
+++ b/printer.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,270 +458,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>adb16565-6da0-4f47-ab26-f2e1ff9ab41f</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>In</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Duable Face</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>20</v>
-      </c>
-      <c r="E2" t="n">
-        <v>15</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2024-09-20</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>21:35:42</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>46cea3b9-bf3a-400c-a9ca-f07bc02c51f0</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Waste</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>paper</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>17:23:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>c0d653bf-2f1a-4cfa-988f-9ee6b267ef45</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Waste</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>paper</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>17:45:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>229acf0c-779f-434d-a864-34fde3ed54e9</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>paper</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>100</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>17:45:52</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>0535ef63-cd48-482b-806e-b8e7360c32ac</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>paper</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>17:51:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1899b5d8-72a6-4f60-91fc-a9c68866dd90</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>paper</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>17:52:14</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>006ffc8f-2e6b-4a91-b27d-4b7a650f632d</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>paper</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>1234</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>17:54:32</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>3d7a2e09-c12c-49df-86b9-f90c2a8fd76f</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Ram</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>10</v>
-      </c>
-      <c r="E9" t="n">
-        <v>10101</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>17:56:11</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add update functionality to the Update button in the printer section
</commit_message>
<xml_diff>
--- a/printer.xlsx
+++ b/printer.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,6 +458,105 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1cf4acd0-85b6-4bfd-967d-e2f3ff3c1165</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Tonore</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>18:11:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>047a14ad-5d3d-4955-b6d1-4295cef09daf</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ram</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>120</v>
+      </c>
+      <c r="E3" t="n">
+        <v>19292</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>18:11:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>482f3d17-ca96-473d-a88f-1cb2edb49201</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Ram</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>19:54:57</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Modify onSelectedItem function to be compatible with the update functionality in the printer section
</commit_message>
<xml_diff>
--- a/printer.xlsx
+++ b/printer.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,6 +557,39 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4e2bd634-bb89-4bc8-881c-f4e64ab9223d</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Duable Face</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>15</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>20:02:45</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add search functionality to the printer section
</commit_message>
<xml_diff>
--- a/printer.xlsx
+++ b/printer.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,6 +590,72 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>0e47dd16-3ece-4c4b-ba97-3101347d82c1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>One Face</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>21:21:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>83cd03f2-981e-4881-9a90-788063c9152b</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Waste</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>21:23:05</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add total calculation feature to the printer section
</commit_message>
<xml_diff>
--- a/printer.xlsx
+++ b/printer.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,7 +560,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4e2bd634-bb89-4bc8-881c-f4e64ab9223d</t>
+          <t>0e47dd16-3ece-4c4b-ba97-3101347d82c1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -570,14 +570,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Duable Face</t>
+          <t>One Face</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="E5" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -586,31 +586,31 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>20:02:45</t>
+          <t>21:21:45</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0e47dd16-3ece-4c4b-ba97-3101347d82c1</t>
+          <t>83cd03f2-981e-4881-9a90-788063c9152b</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>In</t>
+          <t>Waste</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>One Face</t>
+          <t>paper</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>100</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -618,39 +618,6 @@
         </is>
       </c>
       <c r="G6" t="inlineStr">
-        <is>
-          <t>21:21:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>83cd03f2-981e-4881-9a90-788063c9152b</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Waste</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>paper</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>100</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2024-09-23</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
         <is>
           <t>21:23:05</t>
         </is>

</xml_diff>

<commit_message>
Add validation to ensure start date is earlier than end date
</commit_message>
<xml_diff>
--- a/printer.xlsx
+++ b/printer.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,171 +458,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1cf4acd0-85b6-4bfd-967d-e2f3ff3c1165</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Tonore</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2024-09-23</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>18:11:24</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>047a14ad-5d3d-4955-b6d1-4295cef09daf</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Ram</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>120</v>
-      </c>
-      <c r="E3" t="n">
-        <v>19292</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2024-09-23</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>18:11:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>482f3d17-ca96-473d-a88f-1cb2edb49201</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Ram</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2024-09-23</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>19:54:57</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>0e47dd16-3ece-4c4b-ba97-3101347d82c1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>In</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>One Face</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>100</v>
-      </c>
-      <c r="E5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2024-09-23</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>21:21:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>83cd03f2-981e-4881-9a90-788063c9152b</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Waste</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>paper</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>100</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2024-09-23</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>21:23:05</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>